<commit_message>
take constants into account to output
</commit_message>
<xml_diff>
--- a/dataset/models/output/simplified.xlsx
+++ b/dataset/models/output/simplified.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benjaminkauffmann/Desktop/Azasimul/azasimul/dataset/models/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:20001_{0F8A4D6D-DC1D-C840-95E6-13AFD4CA6574}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:20001_{714DAF8A-E5EB-414A-9860-8250BFE35D29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="500" windowWidth="25180" windowHeight="10260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="161">
   <si>
     <t xml:space="preserve">Levelized Cost of Stablized Electricity </t>
   </si>
@@ -543,6 +543,9 @@
   </si>
   <si>
     <t>FOR:[Market.Unskilled Labor + load]</t>
+  </si>
+  <si>
+    <t>[Constants.Dimensions.Length]</t>
   </si>
 </sst>
 </file>
@@ -1511,7 +1514,7 @@
   <dimension ref="A1:AL155"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J51" sqref="J51"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1622,6 +1625,9 @@
       </c>
       <c r="F9" s="34" t="s">
         <v>146</v>
+      </c>
+      <c r="J9" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2973,7 +2979,7 @@
   </sheetPr>
   <dimension ref="C1:X94"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>

</xml_diff>